<commit_message>
Added some basic code structure
</commit_message>
<xml_diff>
--- a/etc/endterm_sheet.xlsx
+++ b/etc/endterm_sheet.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="35">
   <si>
     <t>Närvaro</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>Rekomendation</t>
-  </si>
-  <si>
-    <t>Tränare: William</t>
   </si>
   <si>
     <t>Övrigt</t>
@@ -943,20 +940,20 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" style="8" customWidth="1"/>
-    <col min="2" max="2" width="10" style="8" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="7" style="8" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" style="8" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="8"/>
-    <col min="5" max="5" width="14" style="8" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" style="8" customWidth="1"/>
     <col min="6" max="6" width="5.5703125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="19" style="8" customWidth="1"/>
-    <col min="8" max="8" width="17.5703125" style="8" customWidth="1"/>
-    <col min="9" max="9" width="40.5703125" style="8" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="8" customWidth="1"/>
+    <col min="8" max="8" width="9" style="8" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="8" customWidth="1"/>
     <col min="10" max="10" width="16.140625" style="8" customWidth="1"/>
     <col min="11" max="11" width="22" style="8" customWidth="1"/>
     <col min="12" max="12" width="64" style="8" customWidth="1"/>
@@ -998,301 +995,299 @@
         <v>10</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C2" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="D2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="E2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>18</v>
-      </c>
       <c r="G2" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I2" s="14">
         <v>4</v>
       </c>
       <c r="J2" s="52" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L2" s="16"/>
     </row>
     <row r="3" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="C3" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="D3" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="E3" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="18" t="s">
-        <v>18</v>
-      </c>
       <c r="G3" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3" s="44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I3" s="42">
         <v>3.5</v>
       </c>
       <c r="J3" s="53" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K3" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L3" s="20"/>
     </row>
     <row r="4" spans="1:12" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="C4" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="D4" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="E4" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="18" t="s">
-        <v>18</v>
-      </c>
       <c r="G4" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H4" s="50" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I4" s="43">
         <v>2.5</v>
       </c>
       <c r="J4" s="55" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K4" s="21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L4" s="20"/>
     </row>
     <row r="5" spans="1:12" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="C5" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="D5" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="E5" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="18" t="s">
-        <v>18</v>
-      </c>
       <c r="G5" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H5" s="50" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I5" s="49">
         <v>5</v>
       </c>
       <c r="J5" s="54" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K5" s="21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L5" s="20"/>
     </row>
     <row r="6" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="C6" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="D6" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="E6" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="18" t="s">
-        <v>18</v>
-      </c>
       <c r="G6" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H6" s="44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I6" s="56">
         <v>1</v>
       </c>
       <c r="J6" s="51" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L6" s="20"/>
     </row>
     <row r="7" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="C7" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="D7" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="E7" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="18" t="s">
-        <v>18</v>
-      </c>
       <c r="G7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="45" t="s">
+      <c r="I7" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" s="22" t="s">
         <v>24</v>
-      </c>
-      <c r="I7" s="45" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="51" t="s">
-        <v>30</v>
-      </c>
-      <c r="K7" s="22" t="s">
-        <v>25</v>
       </c>
       <c r="L7" s="20"/>
     </row>
     <row r="8" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="C8" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="D8" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="E8" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="18" t="s">
-        <v>18</v>
-      </c>
       <c r="G8" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H8" s="46" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I8" s="45" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J8" s="51" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K8" s="23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L8" s="20"/>
     </row>
     <row r="9" spans="1:12" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="C9" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>35</v>
-      </c>
       <c r="E9" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="25" t="s">
-        <v>18</v>
-      </c>
       <c r="G9" s="26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H9" s="47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I9" s="48">
         <v>3.5</v>
       </c>
       <c r="J9" s="53" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K9" s="27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L9" s="28"/>
     </row>
     <row r="10" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
-        <v>11</v>
-      </c>
+      <c r="A10" s="29"/>
       <c r="B10" s="30"/>
       <c r="C10" s="30"/>
       <c r="D10" s="30"/>

</xml_diff>